<commit_message>
removed time from fraud and some cleaning
</commit_message>
<xml_diff>
--- a/model-inference/decisionTree/experiments/gpu_profiles/tables/airlinetab.xlsx
+++ b/model-inference/decisionTree/experiments/gpu_profiles/tables/airlinetab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\11\netsdb\model-inference\decisionTree\experiments\gpu_profiles\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF42A715-8D4A-4A6B-AEB5-625714A70F0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913C9F17-FED3-4591-AE6A-C790A205F767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -929,7 +929,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1925,6 +1925,42 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:M24">
     <sortCondition ref="C1:C24"/>
   </sortState>
+  <conditionalFormatting sqref="H2:H24">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F24">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M24">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>